<commit_message>
moved instructions to zip file
</commit_message>
<xml_diff>
--- a/BIO247Project/BIO247ProjectSubmissions/graphs.xlsx
+++ b/BIO247Project/BIO247ProjectSubmissions/graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e56c0a1657867c1/Desktop/BIO247/BIO247Project/BIO247ProjectSubmissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="8_{6E7A3E0E-40E0-4F0B-B0B8-42CFEF61AAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2610837-ED82-4C97-832B-42A2A34EC9DB}"/>
+  <xr:revisionPtr revIDLastSave="179" documentId="8_{6E7A3E0E-40E0-4F0B-B0B8-42CFEF61AAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F2159CB-57FD-4672-90C8-468556FC7F3A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{634B2139-1284-40E4-820A-68D3B13B798C}"/>
+    <workbookView xWindow="8400" yWindow="4320" windowWidth="10125" windowHeight="3300" xr2:uid="{634B2139-1284-40E4-820A-68D3B13B798C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5937,7 +5937,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.51</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10346,8 +10346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512E2B4B-946E-4352-8815-AB02D008CA54}">
   <dimension ref="A1:AG852"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H21" zoomScale="77" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="AL45" sqref="AL45"/>
+    <sheetView tabSelected="1" topLeftCell="H52" zoomScale="77" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="R54" sqref="R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11383,7 +11383,7 @@
         <v>859</v>
       </c>
       <c r="R53">
-        <f>1-R54-R52</f>
+        <f>1-R54-R55</f>
         <v>0.49</v>
       </c>
       <c r="AG53">
@@ -11419,7 +11419,8 @@
         <v>860</v>
       </c>
       <c r="R54">
-        <v>0.51</v>
+        <f>0.51-0.23</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="AG54">
         <v>0.10365853658536579</v>
@@ -11466,6 +11467,10 @@
       </c>
       <c r="L56">
         <v>6.04</v>
+      </c>
+      <c r="R56">
+        <f>SUM(R53:R55)</f>
+        <v>1</v>
       </c>
       <c r="AG56">
         <v>9.1463414634146339E-2</v>

</xml_diff>